<commit_message>
CoursesDT, status and notes
</commit_message>
<xml_diff>
--- a/Processes/ASD_CoursePlanner/Work/Course Planner.xlsx
+++ b/Processes/ASD_CoursePlanner/Work/Course Planner.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <x:si>
     <x:t>Module Name</x:t>
   </x:si>
@@ -135,7 +135,7 @@
     <x:t>Day (8am-6pm)</x:t>
   </x:si>
   <x:si>
-    <x:t>Success</x:t>
+    <x:t>Not processed</x:t>
   </x:si>
   <x:si>
     <x:t>ACCT1101/S2/STLUC/IN/PRA1</x:t>
@@ -249,6 +249,9 @@
     <x:t>EQP - Data Projector (1)
 EQP - Instructor PC
 EQP - Whiteboard (Instructor)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Success</x:t>
   </x:si>
   <x:si>
     <x:t>ECON1120/S2/STLUC/IN/LEC1</x:t>
@@ -1287,7 +1290,7 @@
         <x:v>38</x:v>
       </x:c>
       <x:c r="AA11" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:28">
@@ -1295,7 +1298,7 @@
         <x:v>71</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
         <x:v>30</x:v>
@@ -1337,18 +1340,18 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="P12" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="AA12" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:28">
       <x:c r="A13" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
         <x:v>48</x:v>
@@ -1395,10 +1398,10 @@
     </x:row>
     <x:row r="14" spans="1:28">
       <x:c r="A14" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
         <x:v>30</x:v>
@@ -1448,22 +1451,22 @@
     </x:row>
     <x:row r="15" spans="1:28">
       <x:c r="A15" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
         <x:v>48</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="E15" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
       <x:c r="F15" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="G15" s="1">
         <x:v>0.0833333333333333</x:v>
@@ -1484,33 +1487,33 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="N15" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="P15" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="AA15" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:28">
       <x:c r="A16" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
         <x:v>30</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="E16" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
       <x:c r="F16" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="G16" s="1">
         <x:v>0.0833333333333333</x:v>
@@ -1534,33 +1537,33 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="N16" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="P16" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="AA16" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:28">
       <x:c r="A17" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
         <x:v>35</x:v>
       </x:c>
       <x:c r="F17" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="G17" s="1">
         <x:v>0.375</x:v>
@@ -1581,27 +1584,27 @@
         <x:v>38</x:v>
       </x:c>
       <x:c r="AA17" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:28">
       <x:c r="A18" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="E18" s="0" t="n">
         <x:v>32</x:v>
       </x:c>
       <x:c r="F18" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="G18" s="1">
         <x:v>0.125</x:v>
@@ -1619,30 +1622,30 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="P18" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="AA18" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:28">
       <x:c r="A19" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
         <x:v>41</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="E19" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
       <x:c r="F19" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="G19" s="1">
         <x:v>0.125</x:v>
@@ -1657,10 +1660,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="K19" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="L19" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="M19" s="0" t="s">
         <x:v>67</x:v>
@@ -1671,22 +1674,22 @@
     </x:row>
     <x:row r="20" spans="1:28">
       <x:c r="A20" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
         <x:v>30</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="E20" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="F20" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="G20" s="1">
         <x:v>0.0833333333333333</x:v>
@@ -1701,7 +1704,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="K20" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="L20" s="0" t="s">
         <x:v>35</x:v>
@@ -1715,22 +1718,22 @@
     </x:row>
     <x:row r="21" spans="1:28">
       <x:c r="A21" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
         <x:v>30</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="E21" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
       <x:c r="F21" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="G21" s="1">
         <x:v>0.0833333333333333</x:v>
@@ -1745,7 +1748,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="K21" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="L21" s="0" t="s">
         <x:v>35</x:v>

</xml_diff>